<commit_message>
Updated the attributes and types
</commit_message>
<xml_diff>
--- a/tests/converters/data/goldbeck.xlsx
+++ b/tests/converters/data/goldbeck.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FTL\FTLBank\ipl\data\xlsx\goldbeck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E817B23-FFC5-48A2-9ABD-A1109C777B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D8A409-415C-4CA5-8B1B-89B9E486E590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="114">
   <si>
     <t>ID</t>
   </si>
@@ -61,12 +74,6 @@
     <t>Anzahl Carsharing-Parkplätze</t>
   </si>
   <si>
-    <t>is_supervised</t>
-  </si>
-  <si>
-    <t>is_covered</t>
-  </si>
-  <si>
     <t>Wegeleitsystem</t>
   </si>
   <si>
@@ -149,9 +156,6 @@
   </si>
   <si>
     <t>true</t>
-  </si>
-  <si>
-    <t>Ihr Parkplatz in Deutschland und Österreich | Goldbeck Parking Services (goldbeck-parking.de)</t>
   </si>
   <si>
     <t>Bad Friedrichshall</t>
@@ -351,6 +355,27 @@
   </si>
   <si>
     <t>https://www.goldbeck-parking.de/dauerparken/formular?pu=6855&amp;type=long_term_parking</t>
+  </si>
+  <si>
+    <t>https://www.goldbeck-parking.de</t>
+  </si>
+  <si>
+    <t>Anzahl Ladeplätze</t>
+  </si>
+  <si>
+    <t>Anzahl Frauenparkplätze</t>
+  </si>
+  <si>
+    <t>Anzahl Behindertenparkplätze</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>Überdachung</t>
+  </si>
+  <si>
+    <t>Art der Überwachung</t>
   </si>
 </sst>
 </file>
@@ -358,9 +383,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,6 +397,20 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -409,12 +448,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -717,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP83"/>
+  <dimension ref="A1:AQ83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -737,8 +780,8 @@
     <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="30.7265625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="25.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.08984375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.54296875" bestFit="1" customWidth="1"/>
@@ -757,18 +800,19 @@
     <col min="31" max="31" width="20.6328125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="22.26953125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="79.81640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="29.26953125" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="29.90625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="16.90625" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="79.7265625" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="66.1796875" customWidth="1"/>
+    <col min="41" max="41" width="16" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="23.6328125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="26.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -808,105 +852,112 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AO1" s="1"/>
-      <c r="AP1" s="1"/>
+      <c r="AO1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>110</v>
+      </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F2">
         <v>9.2360277777777764</v>
@@ -915,16 +966,16 @@
         <v>49.211444444444453</v>
       </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K2">
         <v>637</v>
       </c>
       <c r="L2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="N2" t="b">
         <v>0</v>
@@ -960,33 +1011,36 @@
         <v>0</v>
       </c>
       <c r="Z2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="AA2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AH2" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="AK2" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F3">
         <v>9.1355000000000004</v>
@@ -995,96 +1049,99 @@
         <v>48.947583333333327</v>
       </c>
       <c r="H3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K3">
         <v>200</v>
       </c>
       <c r="L3" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" t="b">
+        <v>1</v>
+      </c>
+      <c r="O3" t="b">
+        <v>1</v>
+      </c>
+      <c r="P3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="b">
+        <v>0</v>
+      </c>
+      <c r="R3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S3" t="b">
+        <v>0</v>
+      </c>
+      <c r="T3" t="b">
+        <v>0</v>
+      </c>
+      <c r="U3" t="b">
+        <v>0</v>
+      </c>
+      <c r="V3" t="b">
+        <v>0</v>
+      </c>
+      <c r="X3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA3" t="s">
         <v>48</v>
       </c>
-      <c r="N3" t="b">
-        <v>1</v>
-      </c>
-      <c r="O3" t="b">
-        <v>1</v>
-      </c>
-      <c r="P3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="b">
-        <v>0</v>
-      </c>
-      <c r="R3" t="b">
-        <v>0</v>
-      </c>
-      <c r="S3" t="b">
-        <v>0</v>
-      </c>
-      <c r="T3" t="b">
-        <v>0</v>
-      </c>
-      <c r="U3" t="b">
-        <v>0</v>
-      </c>
-      <c r="V3" t="b">
-        <v>0</v>
-      </c>
-      <c r="X3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y3" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>51</v>
-      </c>
       <c r="AB3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="AC3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="AE3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AF3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="AG3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AH3" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="AK3">
         <v>210</v>
       </c>
+      <c r="AL3" t="s">
+        <v>111</v>
+      </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F4">
         <v>9.0062777777777772</v>
@@ -1093,99 +1150,102 @@
         <v>48.687444444444438</v>
       </c>
       <c r="H4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K4">
         <v>850</v>
       </c>
       <c r="L4" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O4" t="b">
+        <v>1</v>
+      </c>
+      <c r="P4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R4" t="b">
+        <v>0</v>
+      </c>
+      <c r="S4" t="b">
+        <v>1</v>
+      </c>
+      <c r="T4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U4" t="b">
+        <v>1</v>
+      </c>
+      <c r="V4" t="b">
+        <v>0</v>
+      </c>
+      <c r="X4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA4" t="s">
         <v>48</v>
       </c>
-      <c r="N4" t="b">
-        <v>1</v>
-      </c>
-      <c r="O4" t="b">
-        <v>1</v>
-      </c>
-      <c r="P4" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="b">
-        <v>0</v>
-      </c>
-      <c r="R4" t="b">
-        <v>0</v>
-      </c>
-      <c r="S4" t="b">
-        <v>1</v>
-      </c>
-      <c r="T4" t="b">
-        <v>0</v>
-      </c>
-      <c r="U4" t="b">
-        <v>1</v>
-      </c>
-      <c r="V4" t="b">
-        <v>0</v>
-      </c>
-      <c r="X4" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y4" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>51</v>
-      </c>
       <c r="AB4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC4" t="s">
         <v>52</v>
       </c>
-      <c r="AC4" t="s">
-        <v>55</v>
-      </c>
       <c r="AD4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE4" t="s">
         <v>52</v>
       </c>
-      <c r="AE4" t="s">
-        <v>55</v>
-      </c>
       <c r="AF4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AG4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AH4" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="AK4">
         <v>210</v>
       </c>
+      <c r="AL4" t="s">
+        <v>111</v>
+      </c>
       <c r="AM4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F5">
         <v>9.0092499999999998</v>
@@ -1194,93 +1254,96 @@
         <v>48.686611111111112</v>
       </c>
       <c r="H5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="K5">
         <v>102</v>
       </c>
       <c r="L5" t="s">
+        <v>45</v>
+      </c>
+      <c r="N5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O5" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R5" t="b">
+        <v>0</v>
+      </c>
+      <c r="S5" t="b">
+        <v>1</v>
+      </c>
+      <c r="T5" t="b">
+        <v>0</v>
+      </c>
+      <c r="U5" t="b">
+        <v>1</v>
+      </c>
+      <c r="V5" t="b">
+        <v>0</v>
+      </c>
+      <c r="X5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA5" t="s">
         <v>48</v>
       </c>
-      <c r="N5" t="b">
-        <v>1</v>
-      </c>
-      <c r="O5" t="b">
-        <v>0</v>
-      </c>
-      <c r="P5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R5" t="b">
-        <v>0</v>
-      </c>
-      <c r="S5" t="b">
-        <v>1</v>
-      </c>
-      <c r="T5" t="b">
-        <v>0</v>
-      </c>
-      <c r="U5" t="b">
-        <v>1</v>
-      </c>
-      <c r="V5" t="b">
-        <v>0</v>
-      </c>
-      <c r="X5" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>51</v>
-      </c>
       <c r="AB5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC5" t="s">
         <v>52</v>
       </c>
-      <c r="AC5" t="s">
-        <v>55</v>
-      </c>
       <c r="AD5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE5" t="s">
         <v>52</v>
       </c>
-      <c r="AE5" t="s">
-        <v>55</v>
-      </c>
       <c r="AF5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AG5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AH5" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="AK5">
         <v>185</v>
       </c>
+      <c r="AL5" t="s">
+        <v>111</v>
+      </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>92</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F6">
         <v>9.2101666666666659</v>
@@ -1289,16 +1352,16 @@
         <v>49.146472222222222</v>
       </c>
       <c r="H6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K6">
         <v>643</v>
       </c>
       <c r="L6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="N6" t="b">
         <v>1</v>
@@ -1334,33 +1397,36 @@
         <v>0</v>
       </c>
       <c r="Z6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="AA6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AH6" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="AK6" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>111</v>
       </c>
       <c r="AM6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>93</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F7">
         <v>9.1910000000000007</v>
@@ -1369,93 +1435,96 @@
         <v>49.154694444444438</v>
       </c>
       <c r="H7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K7">
         <v>1681</v>
       </c>
       <c r="L7" t="s">
+        <v>45</v>
+      </c>
+      <c r="N7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" t="b">
+        <v>0</v>
+      </c>
+      <c r="P7" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="b">
+        <v>0</v>
+      </c>
+      <c r="R7" t="b">
+        <v>0</v>
+      </c>
+      <c r="S7" t="b">
+        <v>0</v>
+      </c>
+      <c r="T7" t="b">
+        <v>0</v>
+      </c>
+      <c r="U7" t="b">
+        <v>0</v>
+      </c>
+      <c r="V7" t="b">
+        <v>0</v>
+      </c>
+      <c r="X7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y7" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA7" t="s">
         <v>48</v>
       </c>
-      <c r="N7" t="b">
-        <v>0</v>
-      </c>
-      <c r="O7" t="b">
-        <v>0</v>
-      </c>
-      <c r="P7" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q7" t="b">
-        <v>0</v>
-      </c>
-      <c r="R7" t="b">
-        <v>0</v>
-      </c>
-      <c r="S7" t="b">
-        <v>0</v>
-      </c>
-      <c r="T7" t="b">
-        <v>0</v>
-      </c>
-      <c r="U7" t="b">
-        <v>0</v>
-      </c>
-      <c r="V7" t="b">
-        <v>0</v>
-      </c>
-      <c r="X7" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y7" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>51</v>
-      </c>
       <c r="AB7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="AC7" s="2">
         <v>1</v>
       </c>
       <c r="AD7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AE7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AF7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AG7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AH7" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="AK7" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>94</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F8">
         <v>9.2161111111111111</v>
@@ -1464,16 +1533,16 @@
         <v>49.146361111111112</v>
       </c>
       <c r="H8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K8">
         <v>304</v>
       </c>
       <c r="L8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="N8" t="b">
         <v>1</v>
@@ -1509,33 +1578,36 @@
         <v>0</v>
       </c>
       <c r="Z8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="AA8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AH8" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="AK8">
         <v>200</v>
       </c>
+      <c r="AL8" t="s">
+        <v>111</v>
+      </c>
       <c r="AM8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>95</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F9">
         <v>9.2086944444444434</v>
@@ -1544,16 +1616,16 @@
         <v>49.155000000000001</v>
       </c>
       <c r="H9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K9">
         <v>429</v>
       </c>
       <c r="L9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="N9" t="b">
         <v>1</v>
@@ -1589,33 +1661,36 @@
         <v>0</v>
       </c>
       <c r="Z9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="AA9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AH9" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="AK9">
         <v>200</v>
       </c>
+      <c r="AL9" t="s">
+        <v>111</v>
+      </c>
       <c r="AM9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>96</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F10">
         <v>9.2183888888888887</v>
@@ -1624,16 +1699,16 @@
         <v>49.143250000000002</v>
       </c>
       <c r="H10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="I10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="K10">
         <v>78</v>
       </c>
       <c r="L10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="N10" t="b">
         <v>1</v>
@@ -1669,30 +1744,33 @@
         <v>0</v>
       </c>
       <c r="Z10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AA10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AH10" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="AK10">
         <v>200</v>
       </c>
+      <c r="AL10" t="s">
+        <v>111</v>
+      </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>134</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F11">
         <v>8.2077222222222215</v>
@@ -1701,96 +1779,99 @@
         <v>48.857750000000003</v>
       </c>
       <c r="H11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K11">
         <v>380</v>
       </c>
       <c r="L11" t="s">
+        <v>45</v>
+      </c>
+      <c r="N11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O11" t="b">
+        <v>1</v>
+      </c>
+      <c r="P11" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="b">
+        <v>0</v>
+      </c>
+      <c r="R11" t="b">
+        <v>1</v>
+      </c>
+      <c r="S11" t="b">
+        <v>0</v>
+      </c>
+      <c r="T11" t="b">
+        <v>0</v>
+      </c>
+      <c r="U11" t="b">
+        <v>1</v>
+      </c>
+      <c r="V11" t="b">
+        <v>0</v>
+      </c>
+      <c r="X11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y11" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA11" t="s">
         <v>48</v>
       </c>
-      <c r="N11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O11" t="b">
-        <v>1</v>
-      </c>
-      <c r="P11" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="b">
-        <v>0</v>
-      </c>
-      <c r="R11" t="b">
-        <v>1</v>
-      </c>
-      <c r="S11" t="b">
-        <v>0</v>
-      </c>
-      <c r="T11" t="b">
-        <v>0</v>
-      </c>
-      <c r="U11" t="b">
-        <v>1</v>
-      </c>
-      <c r="V11" t="b">
-        <v>0</v>
-      </c>
-      <c r="X11" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y11" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>103</v>
-      </c>
-      <c r="AA11" t="s">
+      <c r="AB11" t="s">
         <v>51</v>
       </c>
-      <c r="AB11" t="s">
-        <v>54</v>
-      </c>
       <c r="AC11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="AD11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AE11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="AF11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AG11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="AH11" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="AK11">
         <v>205</v>
       </c>
+      <c r="AL11" t="s">
+        <v>111</v>
+      </c>
       <c r="AM11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>144</v>
       </c>
       <c r="B12" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C12" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F12">
         <v>7.5966944444444442</v>
@@ -1799,82 +1880,85 @@
         <v>47.591416666666667</v>
       </c>
       <c r="H12" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K12">
         <v>600</v>
       </c>
       <c r="L12" t="s">
+        <v>45</v>
+      </c>
+      <c r="N12" t="b">
+        <v>1</v>
+      </c>
+      <c r="O12" t="b">
+        <v>1</v>
+      </c>
+      <c r="P12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q12" t="b">
+        <v>0</v>
+      </c>
+      <c r="R12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S12" t="b">
+        <v>0</v>
+      </c>
+      <c r="T12" t="b">
+        <v>0</v>
+      </c>
+      <c r="U12" t="b">
+        <v>0</v>
+      </c>
+      <c r="V12" t="b">
+        <v>0</v>
+      </c>
+      <c r="X12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA12" t="s">
         <v>48</v>
       </c>
-      <c r="N12" t="b">
-        <v>1</v>
-      </c>
-      <c r="O12" t="b">
-        <v>1</v>
-      </c>
-      <c r="P12" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q12" t="b">
-        <v>0</v>
-      </c>
-      <c r="R12" t="b">
-        <v>0</v>
-      </c>
-      <c r="S12" t="b">
-        <v>0</v>
-      </c>
-      <c r="T12" t="b">
-        <v>0</v>
-      </c>
-      <c r="U12" t="b">
-        <v>0</v>
-      </c>
-      <c r="V12" t="b">
-        <v>0</v>
-      </c>
-      <c r="X12" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y12" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>108</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>51</v>
-      </c>
       <c r="AB12" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC12" t="s">
         <v>52</v>
       </c>
-      <c r="AC12" t="s">
-        <v>55</v>
-      </c>
       <c r="AD12" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE12" t="s">
         <v>52</v>
       </c>
-      <c r="AE12" t="s">
-        <v>55</v>
-      </c>
       <c r="AF12" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG12" t="s">
         <v>52</v>
       </c>
-      <c r="AG12" t="s">
-        <v>55</v>
-      </c>
       <c r="AH12" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="AK12">
         <v>210</v>
       </c>
+      <c r="AL12" t="s">
+        <v>111</v>
+      </c>
       <c r="AM12" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="31:31" x14ac:dyDescent="0.35">
@@ -1887,5 +1971,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the static data
</commit_message>
<xml_diff>
--- a/tests/converters/data/goldbeck.xlsx
+++ b/tests/converters/data/goldbeck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FTL\FTLBank\ipl\data\xlsx\goldbeck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D8A409-415C-4CA5-8B1B-89B9E486E590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{16950E53-46FC-4134-A64D-9B97CFA5F5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="113">
   <si>
     <t>ID</t>
   </si>
@@ -174,9 +174,6 @@
   </si>
   <si>
     <t>Standardtarif: Bis 20 Minuten kostenlos; Bis 1 Stunde 1,40 €; Jede weitere Stunde 1,40 €; Tageshöchstsatz 8,00 €; Wochenhöchstsatz 28,00 €; Verlorener Parkschein 8,00 €; 7-Tages Ticket (Besucherticket Vorverkauf) 41,00 €</t>
-  </si>
-  <si>
-    <t>kA</t>
   </si>
   <si>
     <t>false</t>
@@ -385,7 +382,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,6 +408,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -445,10 +450,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -458,8 +464,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -763,7 +771,7 @@
   <dimension ref="A1:AQ83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="AL12" sqref="AL12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -853,10 +861,10 @@
         <v>12</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>13</v>
@@ -934,13 +942,13 @@
         <v>37</v>
       </c>
       <c r="AO1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AP1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.35">
@@ -1017,13 +1025,10 @@
         <v>40</v>
       </c>
       <c r="AH2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="AL2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.35">
@@ -1031,10 +1036,10 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
         <v>54</v>
-      </c>
-      <c r="C3" t="s">
-        <v>55</v>
       </c>
       <c r="D3" t="s">
         <v>38</v>
@@ -1049,10 +1054,10 @@
         <v>48.947583333333327</v>
       </c>
       <c r="H3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" t="s">
         <v>56</v>
-      </c>
-      <c r="I3" t="s">
-        <v>57</v>
       </c>
       <c r="K3">
         <v>200</v>
@@ -1094,37 +1099,37 @@
         <v>0</v>
       </c>
       <c r="Z3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB3" t="s">
         <v>58</v>
       </c>
-      <c r="AA3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>59</v>
-      </c>
       <c r="AC3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AD3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AF3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AH3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AK3">
         <v>210</v>
       </c>
       <c r="AL3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.35">
@@ -1132,10 +1137,10 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
         <v>60</v>
-      </c>
-      <c r="C4" t="s">
-        <v>61</v>
       </c>
       <c r="D4" t="s">
         <v>38</v>
@@ -1150,10 +1155,10 @@
         <v>48.687444444444438</v>
       </c>
       <c r="H4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I4" t="s">
         <v>62</v>
-      </c>
-      <c r="I4" t="s">
-        <v>63</v>
       </c>
       <c r="K4">
         <v>850</v>
@@ -1195,40 +1200,40 @@
         <v>0</v>
       </c>
       <c r="Z4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AA4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB4" t="s">
         <v>48</v>
       </c>
-      <c r="AB4" t="s">
-        <v>49</v>
-      </c>
       <c r="AC4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF4" t="s">
         <v>52</v>
       </c>
-      <c r="AD4" t="s">
-        <v>49</v>
-      </c>
-      <c r="AE4" t="s">
+      <c r="AG4" t="s">
         <v>52</v>
       </c>
-      <c r="AF4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>53</v>
-      </c>
       <c r="AH4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AK4">
         <v>210</v>
       </c>
       <c r="AL4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AM4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.35">
@@ -1236,10 +1241,10 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
         <v>38</v>
@@ -1254,10 +1259,10 @@
         <v>48.686611111111112</v>
       </c>
       <c r="H5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" t="s">
         <v>67</v>
-      </c>
-      <c r="I5" t="s">
-        <v>68</v>
       </c>
       <c r="K5">
         <v>102</v>
@@ -1299,37 +1304,37 @@
         <v>0</v>
       </c>
       <c r="Z5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AA5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB5" t="s">
         <v>48</v>
       </c>
-      <c r="AB5" t="s">
-        <v>49</v>
-      </c>
       <c r="AC5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF5" t="s">
         <v>52</v>
       </c>
-      <c r="AD5" t="s">
-        <v>49</v>
-      </c>
-      <c r="AE5" t="s">
+      <c r="AG5" t="s">
         <v>52</v>
       </c>
-      <c r="AF5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>53</v>
-      </c>
       <c r="AH5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AK5">
         <v>185</v>
       </c>
       <c r="AL5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.35">
@@ -1337,10 +1342,10 @@
         <v>92</v>
       </c>
       <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
         <v>72</v>
-      </c>
-      <c r="C6" t="s">
-        <v>73</v>
       </c>
       <c r="E6" t="s">
         <v>39</v>
@@ -1352,10 +1357,10 @@
         <v>49.146472222222222</v>
       </c>
       <c r="H6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" t="s">
         <v>74</v>
-      </c>
-      <c r="I6" t="s">
-        <v>75</v>
       </c>
       <c r="K6">
         <v>643</v>
@@ -1397,22 +1402,19 @@
         <v>0</v>
       </c>
       <c r="Z6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AA6" t="s">
         <v>40</v>
       </c>
       <c r="AH6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="AL6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AM6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.35">
@@ -1420,10 +1422,10 @@
         <v>93</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E7" t="s">
         <v>39</v>
@@ -1435,10 +1437,10 @@
         <v>49.154694444444438</v>
       </c>
       <c r="H7" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" t="s">
         <v>79</v>
-      </c>
-      <c r="I7" t="s">
-        <v>80</v>
       </c>
       <c r="K7">
         <v>1681</v>
@@ -1480,37 +1482,34 @@
         <v>0</v>
       </c>
       <c r="Z7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AA7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AB7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AC7" s="2">
         <v>1</v>
       </c>
       <c r="AD7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AE7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AF7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AG7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AH7" t="s">
-        <v>107</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="AL7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.35">
@@ -1518,10 +1517,10 @@
         <v>94</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E8" t="s">
         <v>39</v>
@@ -1533,10 +1532,10 @@
         <v>49.146361111111112</v>
       </c>
       <c r="H8" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8" t="s">
         <v>83</v>
-      </c>
-      <c r="I8" t="s">
-        <v>84</v>
       </c>
       <c r="K8">
         <v>304</v>
@@ -1578,22 +1577,22 @@
         <v>0</v>
       </c>
       <c r="Z8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AA8" t="s">
         <v>40</v>
       </c>
       <c r="AH8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AK8">
         <v>200</v>
       </c>
       <c r="AL8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AM8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.35">
@@ -1601,10 +1600,10 @@
         <v>95</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E9" t="s">
         <v>39</v>
@@ -1616,10 +1615,10 @@
         <v>49.155000000000001</v>
       </c>
       <c r="H9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I9" t="s">
         <v>88</v>
-      </c>
-      <c r="I9" t="s">
-        <v>89</v>
       </c>
       <c r="K9">
         <v>429</v>
@@ -1661,22 +1660,22 @@
         <v>0</v>
       </c>
       <c r="Z9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AA9" t="s">
         <v>40</v>
       </c>
       <c r="AH9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AK9">
         <v>200</v>
       </c>
       <c r="AL9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AM9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.35">
@@ -1684,10 +1683,10 @@
         <v>96</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E10" t="s">
         <v>39</v>
@@ -1699,10 +1698,10 @@
         <v>49.143250000000002</v>
       </c>
       <c r="H10" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10" t="s">
         <v>93</v>
-      </c>
-      <c r="I10" t="s">
-        <v>94</v>
       </c>
       <c r="K10">
         <v>78</v>
@@ -1744,19 +1743,19 @@
         <v>0</v>
       </c>
       <c r="Z10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AA10" t="s">
         <v>40</v>
       </c>
       <c r="AH10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AK10">
         <v>200</v>
       </c>
       <c r="AL10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.35">
@@ -1764,10 +1763,10 @@
         <v>134</v>
       </c>
       <c r="B11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" t="s">
         <v>96</v>
-      </c>
-      <c r="C11" t="s">
-        <v>97</v>
       </c>
       <c r="E11" t="s">
         <v>39</v>
@@ -1778,11 +1777,11 @@
       <c r="G11">
         <v>48.857750000000003</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="I11" t="s">
         <v>98</v>
-      </c>
-      <c r="I11" t="s">
-        <v>99</v>
       </c>
       <c r="K11">
         <v>380</v>
@@ -1824,40 +1823,40 @@
         <v>0</v>
       </c>
       <c r="Z11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AA11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AB11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AC11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AD11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AE11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AF11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AH11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AK11">
         <v>205</v>
       </c>
       <c r="AL11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AM11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.35">
@@ -1865,10 +1864,10 @@
         <v>144</v>
       </c>
       <c r="B12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E12" t="s">
         <v>39</v>
@@ -1879,11 +1878,11 @@
       <c r="G12">
         <v>47.591416666666667</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="I12" t="s">
         <v>103</v>
-      </c>
-      <c r="I12" t="s">
-        <v>104</v>
       </c>
       <c r="K12">
         <v>600</v>
@@ -1925,40 +1924,40 @@
         <v>0</v>
       </c>
       <c r="Z12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AA12" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB12" t="s">
         <v>48</v>
       </c>
-      <c r="AB12" t="s">
-        <v>49</v>
-      </c>
       <c r="AC12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AD12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AE12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AF12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AG12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AH12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AK12">
         <v>210</v>
       </c>
       <c r="AL12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AM12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="31:31" x14ac:dyDescent="0.35">
@@ -1970,7 +1969,11 @@
       <c r="AG83" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H11" r:id="rId1" xr:uid="{B474EE45-96E7-4523-9B19-D0BDD47F8647}"/>
+    <hyperlink ref="H12" r:id="rId2" xr:uid="{C1C03A49-CB92-446C-80F0-A2D365A58A77}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>